<commit_message>
remove stray value in CL
</commit_message>
<xml_diff>
--- a/e_coli_core_flux.xlsx
+++ b/e_coli_core_flux.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shyam\Documents\Courses\psu\mfa_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA006B67-117F-4F66-871F-D8C6227028B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB482E8-8168-4A81-BA4C-1E22C2D435A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reaction List" sheetId="1" r:id="rId1"/>
@@ -1901,7 +1901,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2268,7 +2268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4997,7 +4997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6034,11 +6034,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CL96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:CE96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BW1" sqref="BW1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6051,7 +6051,7 @@
     <col min="9" max="256" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6298,12 +6298,8 @@
       <c r="CE1" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="CL1" s="1">
-        <f>0.25*J14</f>
-        <v>0.21848037674210774</v>
-      </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -6551,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -6799,7 +6795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -7047,7 +7043,7 @@
         <v>-2.8329717698158102E-28</v>
       </c>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -7295,7 +7291,7 @@
         <v>0.759585463045099</v>
       </c>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -7543,7 +7539,7 @@
         <v>0.759585463045099</v>
       </c>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -7788,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -8036,7 +8032,7 @@
         <v>4.6074289978738099</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -8284,7 +8280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -8532,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -8780,7 +8776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -9025,7 +9021,7 @@
         <v>21.113487235810101</v>
       </c>
     </row>
-    <row r="13" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -9273,7 +9269,7 @@
         <v>63.788053197031701</v>
       </c>
     </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -9518,7 +9514,7 @@
         <v>0.70403694785902304</v>
       </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -9766,7 +9762,7 @@
         <v>-26.641180529154202</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>

</xml_diff>